<commit_message>
Update Maintenance period table.xlsx
</commit_message>
<xml_diff>
--- a/Maintenance period table.xlsx
+++ b/Maintenance period table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lengo\Documents\GitHub\20200303-HelpDesk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{511A4330-5541-4CEC-9961-DE8A0C27089F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09B97D4-8E97-48D6-958A-C4C601CDEEB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{415F967C-83EA-4F3D-9DBA-47E80972D713}"/>
   </bookViews>
@@ -227,9 +227,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -240,6 +237,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,159 +570,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>30</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
         <v>30</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>